<commit_message>
Added controller of checkin improvements
</commit_message>
<xml_diff>
--- a/doc/Pruebas/DatosEntrevistas.xlsx
+++ b/doc/Pruebas/DatosEntrevistas.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paco/Dropbox/Escuela/Profesional/Clases/9º Semestre/Proyecto Integrador/Trabajos/MasterRepo/RonaldMcDonald/doc/Pruebas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{609A955F-F80D-6F46-8C6B-CED72B3267D0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B16B895-DFC5-494C-A445-05555E69C42C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{6317AA5F-36DB-B24A-9F17-5CCC4F4BCEA8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{6317AA5F-36DB-B24A-9F17-5CCC4F4BCEA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$20</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$B$2:$B$20</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t xml:space="preserve">Overall, I am satisfied with how easy it is to use this system  </t>
   </si>
@@ -111,43 +105,46 @@
     <t>User 3</t>
   </si>
   <si>
-    <t>La barra de búsqueda no es fácil de identificar</t>
-  </si>
-  <si>
-    <t>Es fácil encotrar los detalles de cada niño</t>
-  </si>
-  <si>
-    <t>Encontré lo que buscaba rápidamente</t>
-  </si>
-  <si>
-    <t>La interfaz se ve amigable</t>
-  </si>
-  <si>
-    <t>La manera en la que muestra la información es consisa  fácil de entender</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Un poco lento en cargar recursos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muestra que no hay niños y luego carga los niños </t>
-  </si>
-  <si>
-    <t>A veces puede haber mucha información en la página</t>
-  </si>
-  <si>
-    <t>Buscador de niños es útil</t>
-  </si>
-  <si>
-    <t>Interfaz bonita.</t>
-  </si>
-  <si>
-    <t>Fácil de encontrar información común</t>
-  </si>
-  <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>intituitivo</t>
+  </si>
+  <si>
+    <t>rapido</t>
+  </si>
+  <si>
+    <t>facil</t>
+  </si>
+  <si>
+    <t>agradable a la vista</t>
+  </si>
+  <si>
+    <t>sencillo de usar</t>
+  </si>
+  <si>
+    <t>facil de uso</t>
+  </si>
+  <si>
+    <t>comprensible</t>
+  </si>
+  <si>
+    <t>User 4</t>
+  </si>
+  <si>
+    <t>User 5</t>
+  </si>
+  <si>
+    <t>User 6</t>
+  </si>
+  <si>
+    <t>User 7</t>
+  </si>
+  <si>
+    <t>User 8</t>
   </si>
 </sst>
 </file>
@@ -155,9 +152,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,6 +166,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,11 +198,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,61 +376,61 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5.666666666666667</c:v>
+                  <c:v>6.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.333333333333333</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>6.625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.333333333333333</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.333333333333333</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6.875</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1120,16 +1125,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>5685125</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>42663</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>698499</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>563543</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>550842</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>108986</xdr:rowOff>
+      <xdr:rowOff>134386</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1454,10 +1459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE56CC19-3912-9247-B5E5-CFDC4A016B7C}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,12 +1470,12 @@
     <col min="1" max="1" width="102.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -1481,17 +1486,32 @@
       <c r="E1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <f>AVERAGE(C2:E2)</f>
-        <v>5.666666666666667</v>
+        <f>AVERAGE(C2:J2)</f>
+        <v>6.625</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -1499,14 +1519,29 @@
       <c r="E2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <f>AVERAGE(C3:E3)</f>
-        <v>6.666666666666667</v>
+        <f t="shared" ref="B3:B20" si="0">AVERAGE(C3:J3)</f>
+        <v>6.75</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -1517,14 +1552,29 @@
       <c r="E3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <f>AVERAGE(C4:E4)</f>
-        <v>6.666666666666667</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -1535,17 +1585,32 @@
       <c r="E4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <f>AVERAGE(C5:E5)</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>6.75</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -1553,17 +1618,32 @@
       <c r="E5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <f>AVERAGE(C6:E6)</f>
-        <v>6.333333333333333</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -1571,14 +1651,29 @@
       <c r="E6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <f>AVERAGE(C7:E7)</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -1589,14 +1684,29 @@
       <c r="E7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <f>AVERAGE(C8:E8)</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1607,14 +1717,29 @@
       <c r="E8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <f>AVERAGE(C9:E9)</f>
-        <v>6.666666666666667</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -1625,68 +1750,128 @@
       <c r="E9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <f>AVERAGE(C10:E10)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3">
-        <f>AVERAGE(C11:E11)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>6.625</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <f>AVERAGE(C12:E12)</f>
-        <v>4.333333333333333</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <f>AVERAGE(C13:E13)</f>
-        <v>6.333333333333333</v>
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -1697,14 +1882,29 @@
       <c r="E13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <f>AVERAGE(C14:E14)</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -1715,32 +1915,62 @@
       <c r="E14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3">
-        <f>AVERAGE(C15:E15)</f>
-        <v>4.666666666666667</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C15">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <f>AVERAGE(C16:E16)</f>
-        <v>6.666666666666667</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C16">
         <v>7</v>
@@ -1751,13 +1981,28 @@
       <c r="E16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <f>AVERAGE(C17:E17)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C17">
@@ -1769,14 +2014,29 @@
       <c r="E17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <f>AVERAGE(C18:E18)</f>
-        <v>6.666666666666667</v>
+        <f t="shared" si="0"/>
+        <v>6.875</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -1787,17 +2047,32 @@
       <c r="E18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <f>AVERAGE(C19:E19)</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>6.75</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>7</v>
@@ -1805,14 +2080,29 @@
       <c r="E19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="J19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <f>AVERAGE(C20:E20)</f>
-        <v>6.666666666666667</v>
+        <f t="shared" si="0"/>
+        <v>6.75</v>
       </c>
       <c r="C20">
         <v>6</v>
@@ -1823,111 +2113,111 @@
       <c r="E20">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="C30" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A37" s="1"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A39" s="2"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A40" s="2"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="A42" s="2"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="A44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>